<commit_message>
fix rocof equation post-processment
</commit_message>
<xml_diff>
--- a/results/teste.xlsx
+++ b/results/teste.xlsx
@@ -472,7 +472,7 @@
     <col width="19.7109375" customWidth="1" min="11" max="11"/>
     <col width="11.7109375" customWidth="1" min="12" max="12"/>
     <col width="15.7109375" customWidth="1" min="13" max="13"/>
-    <col width="11.7109375" customWidth="1" min="14" max="14"/>
+    <col width="12.7109375" customWidth="1" min="14" max="14"/>
     <col width="11.7109375" customWidth="1" min="15" max="15"/>
     <col width="11.7109375" customWidth="1" min="16" max="16"/>
     <col width="11.7109375" customWidth="1" min="17" max="17"/>
@@ -543,7 +543,7 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>ROCOF</t>
+          <t>ROCOF [Hz/s]</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
@@ -583,10 +583,10 @@
         <v>16.83</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>16.83</v>
       </c>
       <c r="E2" t="n">
-        <v>16.83</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>16.83</v>
@@ -613,16 +613,16 @@
         <v>100.77</v>
       </c>
       <c r="N2" t="n">
-        <v>-159.49</v>
+        <v>-1.33</v>
       </c>
       <c r="O2" t="n">
         <v>1</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R2" t="n">
         <v>1</v>
@@ -642,10 +642,10 @@
         <v>16.68</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>16.68</v>
       </c>
       <c r="E3" t="n">
-        <v>16.68</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
         <v>16.68</v>
@@ -672,16 +672,16 @@
         <v>100.77</v>
       </c>
       <c r="N3" t="n">
-        <v>260.95</v>
+        <v>-1.3</v>
       </c>
       <c r="O3" t="n">
         <v>1</v>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
         <v>1</v>
@@ -701,10 +701,10 @@
         <v>16.18</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>16.18</v>
       </c>
       <c r="E4" t="n">
-        <v>16.18</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
         <v>16.18</v>
@@ -731,16 +731,16 @@
         <v>100.77</v>
       </c>
       <c r="N4" t="n">
-        <v>-419.25</v>
+        <v>-1.28</v>
       </c>
       <c r="O4" t="n">
         <v>1</v>
       </c>
       <c r="P4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4" t="n">
         <v>1</v>
@@ -760,10 +760,10 @@
         <v>15.73</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>15.73</v>
       </c>
       <c r="E5" t="n">
-        <v>15.73</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
         <v>15.73</v>
@@ -790,16 +790,16 @@
         <v>100.77</v>
       </c>
       <c r="N5" t="n">
-        <v>663.34</v>
+        <v>-1.26</v>
       </c>
       <c r="O5" t="n">
         <v>1</v>
       </c>
       <c r="P5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R5" t="n">
         <v>1</v>
@@ -819,10 +819,10 @@
         <v>15.39</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>15.39</v>
       </c>
       <c r="E6" t="n">
-        <v>15.39</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
         <v>15.39</v>
@@ -849,16 +849,16 @@
         <v>100.77</v>
       </c>
       <c r="N6" t="n">
-        <v>-1036.46</v>
+        <v>-1.24</v>
       </c>
       <c r="O6" t="n">
         <v>1</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R6" t="n">
         <v>1</v>
@@ -878,10 +878,10 @@
         <v>15.05</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>15.05</v>
       </c>
       <c r="E7" t="n">
-        <v>15.05</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
         <v>15.05</v>
@@ -908,16 +908,16 @@
         <v>100.77</v>
       </c>
       <c r="N7" t="n">
-        <v>1600.87</v>
+        <v>-1.23</v>
       </c>
       <c r="O7" t="n">
         <v>1</v>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R7" t="n">
         <v>1</v>
@@ -937,10 +937,10 @@
         <v>15.05</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>15.05</v>
       </c>
       <c r="E8" t="n">
-        <v>15.05</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
         <v>15.05</v>
@@ -967,16 +967,16 @@
         <v>100.77</v>
       </c>
       <c r="N8" t="n">
-        <v>-2408.02</v>
+        <v>-1.19</v>
       </c>
       <c r="O8" t="n">
         <v>1</v>
       </c>
       <c r="P8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R8" t="n">
         <v>1</v>
@@ -996,10 +996,10 @@
         <v>15.05</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>15.05</v>
       </c>
       <c r="E9" t="n">
-        <v>15.05</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
         <v>15.05</v>
@@ -1026,16 +1026,16 @@
         <v>100.77</v>
       </c>
       <c r="N9" t="n">
-        <v>3491.4</v>
+        <v>-1.14</v>
       </c>
       <c r="O9" t="n">
         <v>1</v>
       </c>
       <c r="P9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R9" t="n">
         <v>1</v>
@@ -1055,10 +1055,10 @@
         <v>15.05</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>15.05</v>
       </c>
       <c r="E10" t="n">
-        <v>15.05</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
         <v>15.05</v>
@@ -1085,16 +1085,16 @@
         <v>100.77</v>
       </c>
       <c r="N10" t="n">
-        <v>-4872.68</v>
+        <v>-1.1</v>
       </c>
       <c r="O10" t="n">
         <v>1</v>
       </c>
       <c r="P10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R10" t="n">
         <v>1</v>
@@ -1114,10 +1114,10 @@
         <v>15.23</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>15.23</v>
       </c>
       <c r="E11" t="n">
-        <v>15.23</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
         <v>15.23</v>
@@ -1144,16 +1144,16 @@
         <v>100.77</v>
       </c>
       <c r="N11" t="n">
-        <v>6457.72</v>
+        <v>-1.03</v>
       </c>
       <c r="O11" t="n">
         <v>1</v>
       </c>
       <c r="P11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R11" t="n">
         <v>1</v>
@@ -1175,10 +1175,10 @@
         <v>15.62</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>15.62</v>
       </c>
       <c r="E12" t="n">
-        <v>15.62</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
         <v>15.62</v>
@@ -1205,16 +1205,16 @@
         <v>100.77</v>
       </c>
       <c r="N12" t="n">
-        <v>357.84</v>
+        <v>-1.21</v>
       </c>
       <c r="O12" t="n">
         <v>1</v>
       </c>
       <c r="P12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R12" t="n">
         <v>1</v>
@@ -1485,16 +1485,16 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.6</v>
+        <v>-0.53</v>
       </c>
       <c r="G8" t="n">
-        <v>0.8</v>
+        <v>0.73</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.46</v>
+        <v>-0.53</v>
       </c>
       <c r="I8" t="n">
-        <v>0.66</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="9">
@@ -1514,16 +1514,16 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>-0</v>
+        <v>-0.1</v>
       </c>
       <c r="G9" t="n">
-        <v>0.8</v>
+        <v>0.83</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.2</v>
+        <v>-0.1</v>
       </c>
       <c r="I9" t="n">
-        <v>0.85</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="10">
@@ -1543,13 +1543,13 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.2</v>
+        <v>-0.17</v>
       </c>
       <c r="G10" t="n">
         <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.15</v>
+        <v>-0.17</v>
       </c>
       <c r="I10" t="n">
         <v>1</v>
@@ -1612,7 +1612,7 @@
         <v>0.01</v>
       </c>
       <c r="I12" t="n">
-        <v>0.47</v>
+        <v>0.48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
include available inertia in results
</commit_message>
<xml_diff>
--- a/results/teste.xlsx
+++ b/results/teste.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S12"/>
+  <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,11 +473,12 @@
     <col width="11.7109375" customWidth="1" min="12" max="12"/>
     <col width="15.7109375" customWidth="1" min="13" max="13"/>
     <col width="12.7109375" customWidth="1" min="14" max="14"/>
-    <col width="11.7109375" customWidth="1" min="15" max="15"/>
+    <col width="21.7109375" customWidth="1" min="15" max="15"/>
     <col width="11.7109375" customWidth="1" min="16" max="16"/>
     <col width="11.7109375" customWidth="1" min="17" max="17"/>
     <col width="11.7109375" customWidth="1" min="18" max="18"/>
     <col width="11.7109375" customWidth="1" min="19" max="19"/>
+    <col width="11.7109375" customWidth="1" min="20" max="20"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -548,25 +549,30 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
+          <t>Available Inertia [s]</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
           <t>GT1 Status</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>GT2 Status</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>GT3 Status</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>GT4 Status</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>WT1 Status</t>
         </is>
@@ -616,18 +622,21 @@
         <v>-1.33</v>
       </c>
       <c r="O2" t="n">
-        <v>1</v>
+        <v>9.6</v>
       </c>
       <c r="P2" t="n">
         <v>1</v>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -675,18 +684,21 @@
         <v>-1.3</v>
       </c>
       <c r="O3" t="n">
-        <v>1</v>
+        <v>9.6</v>
       </c>
       <c r="P3" t="n">
         <v>1</v>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -734,18 +746,21 @@
         <v>-1.28</v>
       </c>
       <c r="O4" t="n">
-        <v>1</v>
+        <v>9.6</v>
       </c>
       <c r="P4" t="n">
         <v>1</v>
       </c>
       <c r="Q4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
+        <v>1</v>
+      </c>
+      <c r="T4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -793,18 +808,21 @@
         <v>-1.26</v>
       </c>
       <c r="O5" t="n">
-        <v>1</v>
+        <v>9.6</v>
       </c>
       <c r="P5" t="n">
         <v>1</v>
       </c>
       <c r="Q5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -852,18 +870,21 @@
         <v>-1.24</v>
       </c>
       <c r="O6" t="n">
-        <v>1</v>
+        <v>9.6</v>
       </c>
       <c r="P6" t="n">
         <v>1</v>
       </c>
       <c r="Q6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S6" t="n">
+        <v>1</v>
+      </c>
+      <c r="T6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -911,18 +932,21 @@
         <v>-1.23</v>
       </c>
       <c r="O7" t="n">
-        <v>1</v>
+        <v>9.6</v>
       </c>
       <c r="P7" t="n">
         <v>1</v>
       </c>
       <c r="Q7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S7" t="n">
+        <v>1</v>
+      </c>
+      <c r="T7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -970,18 +994,21 @@
         <v>-1.19</v>
       </c>
       <c r="O8" t="n">
-        <v>1</v>
+        <v>9.6</v>
       </c>
       <c r="P8" t="n">
         <v>1</v>
       </c>
       <c r="Q8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S8" t="n">
+        <v>1</v>
+      </c>
+      <c r="T8" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1029,18 +1056,21 @@
         <v>-1.14</v>
       </c>
       <c r="O9" t="n">
-        <v>1</v>
+        <v>9.6</v>
       </c>
       <c r="P9" t="n">
         <v>1</v>
       </c>
       <c r="Q9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S9" t="n">
+        <v>1</v>
+      </c>
+      <c r="T9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1088,18 +1118,21 @@
         <v>-1.1</v>
       </c>
       <c r="O10" t="n">
-        <v>1</v>
+        <v>9.6</v>
       </c>
       <c r="P10" t="n">
         <v>1</v>
       </c>
       <c r="Q10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S10" t="n">
+        <v>1</v>
+      </c>
+      <c r="T10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1147,18 +1180,21 @@
         <v>-1.03</v>
       </c>
       <c r="O11" t="n">
-        <v>1</v>
+        <v>9.6</v>
       </c>
       <c r="P11" t="n">
         <v>1</v>
       </c>
       <c r="Q11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S11" t="n">
+        <v>1</v>
+      </c>
+      <c r="T11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1208,18 +1244,21 @@
         <v>-1.21</v>
       </c>
       <c r="O12" t="n">
-        <v>1</v>
+        <v>9.6</v>
       </c>
       <c r="P12" t="n">
         <v>1</v>
       </c>
       <c r="Q12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S12" t="n">
+        <v>1</v>
+      </c>
+      <c r="T12" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
include wind and storages in rocof formula
</commit_message>
<xml_diff>
--- a/results/teste.xlsx
+++ b/results/teste.xlsx
@@ -586,40 +586,40 @@
         <v>65.5</v>
       </c>
       <c r="C2" t="n">
-        <v>16.83</v>
+        <v>17.12</v>
       </c>
       <c r="D2" t="n">
-        <v>16.83</v>
+        <v>17.12</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>16.83</v>
+        <v>17.12</v>
       </c>
       <c r="G2" t="n">
         <v>13.27</v>
       </c>
       <c r="H2" t="n">
-        <v>1594</v>
+        <v>1602.79</v>
       </c>
       <c r="I2" t="n">
-        <v>15584.27</v>
+        <v>15585.45</v>
       </c>
       <c r="J2" t="n">
-        <v>82.73999999999999</v>
+        <v>83.22</v>
       </c>
       <c r="K2" t="n">
-        <v>808.11</v>
+        <v>808.1799999999999</v>
       </c>
       <c r="L2" t="n">
-        <v>10.86</v>
+        <v>11.04</v>
       </c>
       <c r="M2" t="n">
-        <v>100.77</v>
+        <v>100.78</v>
       </c>
       <c r="N2" t="n">
-        <v>-1.33</v>
+        <v>-0.71</v>
       </c>
       <c r="O2" t="n">
         <v>9.6</v>
@@ -666,22 +666,22 @@
         <v>1589.52</v>
       </c>
       <c r="I3" t="n">
-        <v>15584.27</v>
+        <v>15585.45</v>
       </c>
       <c r="J3" t="n">
         <v>82.48999999999999</v>
       </c>
       <c r="K3" t="n">
-        <v>808.11</v>
+        <v>808.1799999999999</v>
       </c>
       <c r="L3" t="n">
         <v>10.76</v>
       </c>
       <c r="M3" t="n">
-        <v>100.77</v>
+        <v>100.78</v>
       </c>
       <c r="N3" t="n">
-        <v>-1.3</v>
+        <v>-0.7</v>
       </c>
       <c r="O3" t="n">
         <v>9.6</v>
@@ -728,22 +728,22 @@
         <v>1574.61</v>
       </c>
       <c r="I4" t="n">
-        <v>15584.27</v>
+        <v>15585.45</v>
       </c>
       <c r="J4" t="n">
         <v>81.68000000000001</v>
       </c>
       <c r="K4" t="n">
-        <v>808.11</v>
+        <v>808.1799999999999</v>
       </c>
       <c r="L4" t="n">
         <v>10.44</v>
       </c>
       <c r="M4" t="n">
-        <v>100.77</v>
+        <v>100.78</v>
       </c>
       <c r="N4" t="n">
-        <v>-1.28</v>
+        <v>-0.67</v>
       </c>
       <c r="O4" t="n">
         <v>9.6</v>
@@ -790,22 +790,22 @@
         <v>1561.33</v>
       </c>
       <c r="I5" t="n">
-        <v>15584.27</v>
+        <v>15585.45</v>
       </c>
       <c r="J5" t="n">
         <v>80.95999999999999</v>
       </c>
       <c r="K5" t="n">
-        <v>808.11</v>
+        <v>808.1799999999999</v>
       </c>
       <c r="L5" t="n">
         <v>10.15</v>
       </c>
       <c r="M5" t="n">
-        <v>100.77</v>
+        <v>100.78</v>
       </c>
       <c r="N5" t="n">
-        <v>-1.26</v>
+        <v>-0.66</v>
       </c>
       <c r="O5" t="n">
         <v>9.6</v>
@@ -852,22 +852,22 @@
         <v>1551.59</v>
       </c>
       <c r="I6" t="n">
-        <v>15584.27</v>
+        <v>15585.45</v>
       </c>
       <c r="J6" t="n">
         <v>80.44</v>
       </c>
       <c r="K6" t="n">
-        <v>808.11</v>
+        <v>808.1799999999999</v>
       </c>
       <c r="L6" t="n">
         <v>9.93</v>
       </c>
       <c r="M6" t="n">
-        <v>100.77</v>
+        <v>100.78</v>
       </c>
       <c r="N6" t="n">
-        <v>-1.24</v>
+        <v>-0.64</v>
       </c>
       <c r="O6" t="n">
         <v>9.6</v>
@@ -896,40 +896,40 @@
         <v>59.61</v>
       </c>
       <c r="C7" t="n">
-        <v>15.05</v>
+        <v>15.04</v>
       </c>
       <c r="D7" t="n">
-        <v>15.05</v>
+        <v>15.04</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>15.05</v>
+        <v>15.04</v>
       </c>
       <c r="G7" t="n">
         <v>14.48</v>
       </c>
       <c r="H7" t="n">
-        <v>1541.57</v>
+        <v>1541.54</v>
       </c>
       <c r="I7" t="n">
-        <v>15584.27</v>
+        <v>15585.45</v>
       </c>
       <c r="J7" t="n">
         <v>79.90000000000001</v>
       </c>
       <c r="K7" t="n">
-        <v>808.11</v>
+        <v>808.1799999999999</v>
       </c>
       <c r="L7" t="n">
         <v>9.699999999999999</v>
       </c>
       <c r="M7" t="n">
-        <v>100.77</v>
+        <v>100.78</v>
       </c>
       <c r="N7" t="n">
-        <v>-1.23</v>
+        <v>-0.63</v>
       </c>
       <c r="O7" t="n">
         <v>9.6</v>
@@ -958,40 +958,40 @@
         <v>58.56</v>
       </c>
       <c r="C8" t="n">
-        <v>15.05</v>
+        <v>14.95</v>
       </c>
       <c r="D8" t="n">
-        <v>15.05</v>
+        <v>14.95</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>15.05</v>
+        <v>14.95</v>
       </c>
       <c r="G8" t="n">
         <v>14.48</v>
       </c>
       <c r="H8" t="n">
-        <v>1541.59</v>
+        <v>1538.74</v>
       </c>
       <c r="I8" t="n">
-        <v>15584.27</v>
+        <v>15585.45</v>
       </c>
       <c r="J8" t="n">
-        <v>79.90000000000001</v>
+        <v>79.75</v>
       </c>
       <c r="K8" t="n">
-        <v>808.11</v>
+        <v>808.1799999999999</v>
       </c>
       <c r="L8" t="n">
-        <v>9.699999999999999</v>
+        <v>9.640000000000001</v>
       </c>
       <c r="M8" t="n">
-        <v>100.77</v>
+        <v>100.78</v>
       </c>
       <c r="N8" t="n">
-        <v>-1.19</v>
+        <v>-0.62</v>
       </c>
       <c r="O8" t="n">
         <v>9.6</v>
@@ -1020,40 +1020,40 @@
         <v>57.51</v>
       </c>
       <c r="C9" t="n">
-        <v>15.05</v>
+        <v>14.98</v>
       </c>
       <c r="D9" t="n">
-        <v>15.05</v>
+        <v>14.98</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>15.05</v>
+        <v>14.98</v>
       </c>
       <c r="G9" t="n">
         <v>12.57</v>
       </c>
       <c r="H9" t="n">
-        <v>1541.62</v>
+        <v>1539.74</v>
       </c>
       <c r="I9" t="n">
-        <v>15584.27</v>
+        <v>15585.45</v>
       </c>
       <c r="J9" t="n">
-        <v>79.90000000000001</v>
+        <v>79.8</v>
       </c>
       <c r="K9" t="n">
-        <v>808.11</v>
+        <v>808.1799999999999</v>
       </c>
       <c r="L9" t="n">
-        <v>9.710000000000001</v>
+        <v>9.66</v>
       </c>
       <c r="M9" t="n">
-        <v>100.77</v>
+        <v>100.78</v>
       </c>
       <c r="N9" t="n">
-        <v>-1.14</v>
+        <v>-0.62</v>
       </c>
       <c r="O9" t="n">
         <v>9.6</v>
@@ -1082,40 +1082,40 @@
         <v>56.46</v>
       </c>
       <c r="C10" t="n">
-        <v>15.05</v>
+        <v>14.95</v>
       </c>
       <c r="D10" t="n">
-        <v>15.05</v>
+        <v>14.95</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>15.05</v>
+        <v>14.95</v>
       </c>
       <c r="G10" t="n">
         <v>11.66</v>
       </c>
       <c r="H10" t="n">
-        <v>1541.64</v>
+        <v>1538.79</v>
       </c>
       <c r="I10" t="n">
-        <v>15584.27</v>
+        <v>15585.45</v>
       </c>
       <c r="J10" t="n">
-        <v>79.90000000000001</v>
+        <v>79.75</v>
       </c>
       <c r="K10" t="n">
-        <v>808.11</v>
+        <v>808.1799999999999</v>
       </c>
       <c r="L10" t="n">
-        <v>9.710000000000001</v>
+        <v>9.640000000000001</v>
       </c>
       <c r="M10" t="n">
-        <v>100.77</v>
+        <v>100.78</v>
       </c>
       <c r="N10" t="n">
-        <v>-1.1</v>
+        <v>-0.62</v>
       </c>
       <c r="O10" t="n">
         <v>9.6</v>
@@ -1162,22 +1162,22 @@
         <v>1546.81</v>
       </c>
       <c r="I11" t="n">
-        <v>15584.27</v>
+        <v>15585.45</v>
       </c>
       <c r="J11" t="n">
         <v>80.18000000000001</v>
       </c>
       <c r="K11" t="n">
-        <v>808.11</v>
+        <v>808.1799999999999</v>
       </c>
       <c r="L11" t="n">
         <v>9.82</v>
       </c>
       <c r="M11" t="n">
-        <v>100.77</v>
+        <v>100.78</v>
       </c>
       <c r="N11" t="n">
-        <v>-1.03</v>
+        <v>-0.63</v>
       </c>
       <c r="O11" t="n">
         <v>9.6</v>
@@ -1208,40 +1208,40 @@
         <v>60.27</v>
       </c>
       <c r="C12" t="n">
-        <v>15.62</v>
+        <v>15.63</v>
       </c>
       <c r="D12" t="n">
-        <v>15.62</v>
+        <v>15.63</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>15.62</v>
+        <v>15.63</v>
       </c>
       <c r="G12" t="n">
         <v>13.39</v>
       </c>
       <c r="H12" t="n">
-        <v>1558.43</v>
+        <v>1558.54</v>
       </c>
       <c r="I12" t="n">
-        <v>15584.27</v>
+        <v>15585.45</v>
       </c>
       <c r="J12" t="n">
-        <v>80.81</v>
+        <v>80.81999999999999</v>
       </c>
       <c r="K12" t="n">
-        <v>808.11</v>
+        <v>808.1799999999999</v>
       </c>
       <c r="L12" t="n">
         <v>10.08</v>
       </c>
       <c r="M12" t="n">
-        <v>100.77</v>
+        <v>100.78</v>
       </c>
       <c r="N12" t="n">
-        <v>-1.21</v>
+        <v>-0.65</v>
       </c>
       <c r="O12" t="n">
         <v>9.6</v>
@@ -1273,7 +1273,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1287,8 +1287,6 @@
     <col width="16" customWidth="1" min="5" max="5"/>
     <col width="15" customWidth="1" min="6" max="6"/>
     <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1322,16 +1320,6 @@
           <t>ST1 SOC [MWh]</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
-        <is>
-          <t>ST2 [MW]</t>
-        </is>
-      </c>
-      <c r="I1" s="2" t="inlineStr">
-        <is>
-          <t>ST2 SOC [MWh]</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -1341,7 +1329,7 @@
         <v>65.5</v>
       </c>
       <c r="C2" t="n">
-        <v>50.49</v>
+        <v>51.36</v>
       </c>
       <c r="D2" t="n">
         <v>13.27</v>
@@ -1355,12 +1343,6 @@
       <c r="G2" t="n">
         <v>0.2</v>
       </c>
-      <c r="H2" t="n">
-        <v>0.87</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -1382,12 +1364,6 @@
         <v>-0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="H3" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I3" t="n">
         <v>0.2</v>
       </c>
     </row>
@@ -1413,12 +1389,6 @@
       <c r="G4" t="n">
         <v>0.2</v>
       </c>
-      <c r="H4" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -1442,12 +1412,6 @@
       <c r="G5" t="n">
         <v>0.2</v>
       </c>
-      <c r="H5" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -1471,12 +1435,6 @@
       <c r="G6" t="n">
         <v>0.2</v>
       </c>
-      <c r="H6" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -1486,7 +1444,7 @@
         <v>59.61</v>
       </c>
       <c r="C7" t="n">
-        <v>45.14</v>
+        <v>45.13</v>
       </c>
       <c r="D7" t="n">
         <v>14.48</v>
@@ -1498,12 +1456,6 @@
         <v>-0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="H7" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I7" t="n">
         <v>0.2</v>
       </c>
     </row>
@@ -1515,7 +1467,7 @@
         <v>58.56</v>
       </c>
       <c r="C8" t="n">
-        <v>45.14</v>
+        <v>44.84</v>
       </c>
       <c r="D8" t="n">
         <v>14.48</v>
@@ -1524,16 +1476,10 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.53</v>
+        <v>-0.75</v>
       </c>
       <c r="G8" t="n">
-        <v>0.73</v>
-      </c>
-      <c r="H8" t="n">
-        <v>-0.53</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.73</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="9">
@@ -1544,7 +1490,7 @@
         <v>57.51</v>
       </c>
       <c r="C9" t="n">
-        <v>45.14</v>
+        <v>44.94</v>
       </c>
       <c r="D9" t="n">
         <v>12.57</v>
@@ -1553,16 +1499,10 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.1</v>
+        <v>-0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.83</v>
-      </c>
-      <c r="H9" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.83</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="10">
@@ -1573,7 +1513,7 @@
         <v>56.46</v>
       </c>
       <c r="C10" t="n">
-        <v>45.14</v>
+        <v>44.84</v>
       </c>
       <c r="D10" t="n">
         <v>11.66</v>
@@ -1582,15 +1522,9 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.17</v>
+        <v>-0.05</v>
       </c>
       <c r="G10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" t="n">
-        <v>-0.17</v>
-      </c>
-      <c r="I10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1616,12 +1550,6 @@
       <c r="G11" t="n">
         <v>1</v>
       </c>
-      <c r="H11" t="n">
-        <v>-0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
@@ -1633,7 +1561,7 @@
         <v>60.27</v>
       </c>
       <c r="C12" t="n">
-        <v>46.87</v>
+        <v>46.88</v>
       </c>
       <c r="D12" t="n">
         <v>13.39</v>
@@ -1645,13 +1573,7 @@
         <v>0.01</v>
       </c>
       <c r="G12" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix reserve and delta P save functions
</commit_message>
<xml_diff>
--- a/results/teste.xlsx
+++ b/results/teste.xlsx
@@ -604,58 +604,58 @@
         <v>65.5</v>
       </c>
       <c r="C2" t="n">
-        <v>12.84</v>
+        <v>13.9</v>
       </c>
       <c r="D2" t="n">
-        <v>12.84</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>12.84</v>
+        <v>13.9</v>
       </c>
       <c r="F2" t="n">
-        <v>12.84</v>
+        <v>13.9</v>
       </c>
       <c r="G2" t="n">
-        <v>13.27</v>
+        <v>22.92</v>
       </c>
       <c r="H2" t="n">
-        <v>1974.28</v>
+        <v>1509.48</v>
       </c>
       <c r="I2" t="n">
-        <v>19352.98</v>
+        <v>14866.68</v>
       </c>
       <c r="J2" t="n">
-        <v>102.21</v>
+        <v>78.18000000000001</v>
       </c>
       <c r="K2" t="n">
-        <v>1001.49</v>
+        <v>769.73</v>
       </c>
       <c r="L2" t="n">
-        <v>11.04</v>
+        <v>8.970000000000001</v>
       </c>
       <c r="M2" t="n">
-        <v>100.78</v>
+        <v>84.22</v>
       </c>
       <c r="N2" t="n">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="O2" t="n">
-        <v>12.8</v>
+        <v>9.6</v>
       </c>
       <c r="P2" t="n">
-        <v>38.64</v>
+        <v>25.8</v>
       </c>
       <c r="Q2" t="n">
-        <v>19.94</v>
+        <v>10.36</v>
       </c>
       <c r="R2" t="n">
-        <v>38.64</v>
+        <v>3.3</v>
       </c>
       <c r="S2" t="n">
         <v>1</v>
       </c>
       <c r="T2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U2" t="n">
         <v>1</v>
@@ -675,58 +675,58 @@
         <v>64.52</v>
       </c>
       <c r="C3" t="n">
-        <v>12.51</v>
+        <v>13.98</v>
       </c>
       <c r="D3" t="n">
-        <v>12.51</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>12.51</v>
+        <v>13.98</v>
       </c>
       <c r="F3" t="n">
-        <v>12.51</v>
+        <v>13.98</v>
       </c>
       <c r="G3" t="n">
-        <v>14.48</v>
+        <v>22.58</v>
       </c>
       <c r="H3" t="n">
-        <v>1962.65</v>
+        <v>1511.63</v>
       </c>
       <c r="I3" t="n">
-        <v>19352.98</v>
+        <v>14866.68</v>
       </c>
       <c r="J3" t="n">
-        <v>101.59</v>
+        <v>78.3</v>
       </c>
       <c r="K3" t="n">
-        <v>1001.49</v>
+        <v>769.73</v>
       </c>
       <c r="L3" t="n">
-        <v>10.76</v>
+        <v>9.02</v>
       </c>
       <c r="M3" t="n">
-        <v>100.78</v>
+        <v>84.22</v>
       </c>
       <c r="N3" t="n">
-        <v>0.64</v>
+        <v>0.48</v>
       </c>
       <c r="O3" t="n">
-        <v>12.8</v>
+        <v>9.6</v>
       </c>
       <c r="P3" t="n">
-        <v>39.96</v>
+        <v>25.56</v>
       </c>
       <c r="Q3" t="n">
-        <v>20.46</v>
+        <v>10.3</v>
       </c>
       <c r="R3" t="n">
-        <v>39.96</v>
+        <v>3.06</v>
       </c>
       <c r="S3" t="n">
         <v>1</v>
       </c>
       <c r="T3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U3" t="n">
         <v>1</v>
@@ -746,58 +746,58 @@
         <v>63.02</v>
       </c>
       <c r="C4" t="n">
-        <v>12.14</v>
+        <v>13.65</v>
       </c>
       <c r="D4" t="n">
-        <v>12.14</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>12.14</v>
+        <v>13.65</v>
       </c>
       <c r="F4" t="n">
-        <v>12.14</v>
+        <v>13.65</v>
       </c>
       <c r="G4" t="n">
-        <v>14.48</v>
+        <v>22.06</v>
       </c>
       <c r="H4" t="n">
-        <v>1949.54</v>
+        <v>1502.69</v>
       </c>
       <c r="I4" t="n">
-        <v>19352.98</v>
+        <v>14866.68</v>
       </c>
       <c r="J4" t="n">
-        <v>100.9</v>
+        <v>77.81999999999999</v>
       </c>
       <c r="K4" t="n">
-        <v>1001.49</v>
+        <v>769.73</v>
       </c>
       <c r="L4" t="n">
-        <v>10.44</v>
+        <v>8.81</v>
       </c>
       <c r="M4" t="n">
-        <v>100.78</v>
+        <v>84.22</v>
       </c>
       <c r="N4" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.54</v>
       </c>
       <c r="O4" t="n">
-        <v>12.8</v>
+        <v>9.6</v>
       </c>
       <c r="P4" t="n">
-        <v>41.45</v>
+        <v>26.54</v>
       </c>
       <c r="Q4" t="n">
-        <v>21.09</v>
+        <v>10.55</v>
       </c>
       <c r="R4" t="n">
-        <v>41.45</v>
+        <v>4.04</v>
       </c>
       <c r="S4" t="n">
         <v>1</v>
       </c>
       <c r="T4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4" t="n">
         <v>1</v>
@@ -817,58 +817,58 @@
         <v>61.66</v>
       </c>
       <c r="C5" t="n">
-        <v>11.8</v>
+        <v>13.36</v>
       </c>
       <c r="D5" t="n">
-        <v>11.8</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>11.8</v>
+        <v>13.36</v>
       </c>
       <c r="F5" t="n">
-        <v>11.8</v>
+        <v>13.36</v>
       </c>
       <c r="G5" t="n">
-        <v>14.48</v>
+        <v>21.58</v>
       </c>
       <c r="H5" t="n">
-        <v>1937.81</v>
+        <v>1494.7</v>
       </c>
       <c r="I5" t="n">
-        <v>19352.98</v>
+        <v>14866.68</v>
       </c>
       <c r="J5" t="n">
-        <v>100.28</v>
+        <v>77.40000000000001</v>
       </c>
       <c r="K5" t="n">
-        <v>1001.49</v>
+        <v>769.73</v>
       </c>
       <c r="L5" t="n">
-        <v>10.15</v>
+        <v>8.619999999999999</v>
       </c>
       <c r="M5" t="n">
-        <v>100.78</v>
+        <v>84.22</v>
       </c>
       <c r="N5" t="n">
-        <v>0.73</v>
+        <v>0.59</v>
       </c>
       <c r="O5" t="n">
-        <v>12.8</v>
+        <v>9.6</v>
       </c>
       <c r="P5" t="n">
-        <v>42.81</v>
+        <v>27.42</v>
       </c>
       <c r="Q5" t="n">
-        <v>21.7</v>
+        <v>10.78</v>
       </c>
       <c r="R5" t="n">
-        <v>42.81</v>
+        <v>4.92</v>
       </c>
       <c r="S5" t="n">
         <v>1</v>
       </c>
       <c r="T5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U5" t="n">
         <v>1</v>
@@ -888,58 +888,58 @@
         <v>60.66</v>
       </c>
       <c r="C6" t="n">
-        <v>11.55</v>
+        <v>13.14</v>
       </c>
       <c r="D6" t="n">
-        <v>11.55</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>11.55</v>
+        <v>13.14</v>
       </c>
       <c r="F6" t="n">
-        <v>11.55</v>
+        <v>13.14</v>
       </c>
       <c r="G6" t="n">
-        <v>14.48</v>
+        <v>21.23</v>
       </c>
       <c r="H6" t="n">
-        <v>1929.2</v>
+        <v>1488.81</v>
       </c>
       <c r="I6" t="n">
-        <v>19352.98</v>
+        <v>14866.68</v>
       </c>
       <c r="J6" t="n">
-        <v>99.83</v>
+        <v>77.08</v>
       </c>
       <c r="K6" t="n">
-        <v>1001.49</v>
+        <v>769.73</v>
       </c>
       <c r="L6" t="n">
-        <v>9.93</v>
+        <v>8.48</v>
       </c>
       <c r="M6" t="n">
-        <v>100.78</v>
+        <v>84.22</v>
       </c>
       <c r="N6" t="n">
-        <v>0.76</v>
+        <v>0.62</v>
       </c>
       <c r="O6" t="n">
-        <v>12.8</v>
+        <v>9.6</v>
       </c>
       <c r="P6" t="n">
-        <v>43.82</v>
+        <v>28.07</v>
       </c>
       <c r="Q6" t="n">
-        <v>22.17</v>
+        <v>10.96</v>
       </c>
       <c r="R6" t="n">
-        <v>43.82</v>
+        <v>5.57</v>
       </c>
       <c r="S6" t="n">
         <v>1</v>
       </c>
       <c r="T6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U6" t="n">
         <v>1</v>
@@ -959,58 +959,58 @@
         <v>59.61</v>
       </c>
       <c r="C7" t="n">
-        <v>11.28</v>
+        <v>12.92</v>
       </c>
       <c r="D7" t="n">
-        <v>11.28</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>11.28</v>
+        <v>12.92</v>
       </c>
       <c r="F7" t="n">
-        <v>11.28</v>
+        <v>12.92</v>
       </c>
       <c r="G7" t="n">
-        <v>14.48</v>
+        <v>20.86</v>
       </c>
       <c r="H7" t="n">
-        <v>1920.28</v>
+        <v>1482.71</v>
       </c>
       <c r="I7" t="n">
-        <v>19352.98</v>
+        <v>14866.68</v>
       </c>
       <c r="J7" t="n">
-        <v>99.36</v>
+        <v>76.76000000000001</v>
       </c>
       <c r="K7" t="n">
-        <v>1001.49</v>
+        <v>769.73</v>
       </c>
       <c r="L7" t="n">
-        <v>9.699999999999999</v>
+        <v>8.33</v>
       </c>
       <c r="M7" t="n">
-        <v>100.78</v>
+        <v>84.22</v>
       </c>
       <c r="N7" t="n">
-        <v>0.79</v>
+        <v>0.66</v>
       </c>
       <c r="O7" t="n">
-        <v>12.8</v>
+        <v>9.6</v>
       </c>
       <c r="P7" t="n">
-        <v>44.87</v>
+        <v>28.75</v>
       </c>
       <c r="Q7" t="n">
-        <v>22.69</v>
+        <v>11.15</v>
       </c>
       <c r="R7" t="n">
-        <v>44.87</v>
+        <v>6.25</v>
       </c>
       <c r="S7" t="n">
         <v>1</v>
       </c>
       <c r="T7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U7" t="n">
         <v>1</v>
@@ -1030,58 +1030,58 @@
         <v>58.56</v>
       </c>
       <c r="C8" t="n">
-        <v>11.21</v>
+        <v>12.69</v>
       </c>
       <c r="D8" t="n">
-        <v>11.21</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>11.21</v>
+        <v>12.69</v>
       </c>
       <c r="F8" t="n">
-        <v>11.21</v>
+        <v>12.69</v>
       </c>
       <c r="G8" t="n">
-        <v>14.48</v>
+        <v>20.5</v>
       </c>
       <c r="H8" t="n">
-        <v>1917.78</v>
+        <v>1476.65</v>
       </c>
       <c r="I8" t="n">
-        <v>19352.98</v>
+        <v>14866.68</v>
       </c>
       <c r="J8" t="n">
-        <v>99.23</v>
+        <v>76.44</v>
       </c>
       <c r="K8" t="n">
-        <v>1001.49</v>
+        <v>769.73</v>
       </c>
       <c r="L8" t="n">
-        <v>9.640000000000001</v>
+        <v>8.18</v>
       </c>
       <c r="M8" t="n">
-        <v>100.78</v>
+        <v>84.22</v>
       </c>
       <c r="N8" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="O8" t="n">
-        <v>12.8</v>
+        <v>9.6</v>
       </c>
       <c r="P8" t="n">
-        <v>45.16</v>
+        <v>29.44</v>
       </c>
       <c r="Q8" t="n">
-        <v>22.84</v>
+        <v>11.35</v>
       </c>
       <c r="R8" t="n">
-        <v>45.16</v>
+        <v>6.94</v>
       </c>
       <c r="S8" t="n">
         <v>1</v>
       </c>
       <c r="T8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U8" t="n">
         <v>1</v>
@@ -1101,58 +1101,58 @@
         <v>57.51</v>
       </c>
       <c r="C9" t="n">
-        <v>11.24</v>
+        <v>12.46</v>
       </c>
       <c r="D9" t="n">
-        <v>11.24</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>11.24</v>
+        <v>12.46</v>
       </c>
       <c r="F9" t="n">
-        <v>11.24</v>
+        <v>12.46</v>
       </c>
       <c r="G9" t="n">
-        <v>12.57</v>
+        <v>20.13</v>
       </c>
       <c r="H9" t="n">
-        <v>1918.67</v>
+        <v>1470.64</v>
       </c>
       <c r="I9" t="n">
-        <v>19352.98</v>
+        <v>14866.68</v>
       </c>
       <c r="J9" t="n">
-        <v>99.27</v>
+        <v>76.12</v>
       </c>
       <c r="K9" t="n">
-        <v>1001.49</v>
+        <v>769.73</v>
       </c>
       <c r="L9" t="n">
-        <v>9.66</v>
+        <v>8.039999999999999</v>
       </c>
       <c r="M9" t="n">
-        <v>100.78</v>
+        <v>84.22</v>
       </c>
       <c r="N9" t="n">
-        <v>0.79</v>
+        <v>0.74</v>
       </c>
       <c r="O9" t="n">
-        <v>12.8</v>
+        <v>9.6</v>
       </c>
       <c r="P9" t="n">
-        <v>45.06</v>
+        <v>30.12</v>
       </c>
       <c r="Q9" t="n">
-        <v>22.78</v>
+        <v>11.56</v>
       </c>
       <c r="R9" t="n">
-        <v>45.06</v>
+        <v>7.62</v>
       </c>
       <c r="S9" t="n">
         <v>1</v>
       </c>
       <c r="T9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U9" t="n">
         <v>1</v>
@@ -1172,58 +1172,58 @@
         <v>56.46</v>
       </c>
       <c r="C10" t="n">
-        <v>11.21</v>
+        <v>12.23</v>
       </c>
       <c r="D10" t="n">
-        <v>11.21</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>11.21</v>
+        <v>12.23</v>
       </c>
       <c r="F10" t="n">
-        <v>11.21</v>
+        <v>12.23</v>
       </c>
       <c r="G10" t="n">
-        <v>11.66</v>
+        <v>19.76</v>
       </c>
       <c r="H10" t="n">
-        <v>1917.84</v>
+        <v>1464.67</v>
       </c>
       <c r="I10" t="n">
-        <v>19352.98</v>
+        <v>14866.68</v>
       </c>
       <c r="J10" t="n">
-        <v>99.23</v>
+        <v>75.81</v>
       </c>
       <c r="K10" t="n">
-        <v>1001.49</v>
+        <v>769.73</v>
       </c>
       <c r="L10" t="n">
-        <v>9.640000000000001</v>
+        <v>7.89</v>
       </c>
       <c r="M10" t="n">
-        <v>100.78</v>
+        <v>84.22</v>
       </c>
       <c r="N10" t="n">
-        <v>0.8</v>
+        <v>0.77</v>
       </c>
       <c r="O10" t="n">
-        <v>12.8</v>
+        <v>9.6</v>
       </c>
       <c r="P10" t="n">
-        <v>45.16</v>
+        <v>30.8</v>
       </c>
       <c r="Q10" t="n">
-        <v>22.83</v>
+        <v>11.77</v>
       </c>
       <c r="R10" t="n">
-        <v>45.16</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="S10" t="n">
         <v>1</v>
       </c>
       <c r="T10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U10" t="n">
         <v>1</v>
@@ -1243,58 +1243,58 @@
         <v>55.23</v>
       </c>
       <c r="C11" t="n">
-        <v>11.42</v>
+        <v>12.23</v>
       </c>
       <c r="D11" t="n">
-        <v>11.42</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>11.42</v>
+        <v>12.23</v>
       </c>
       <c r="F11" t="n">
-        <v>11.42</v>
+        <v>12.23</v>
       </c>
       <c r="G11" t="n">
-        <v>9.550000000000001</v>
+        <v>19.33</v>
       </c>
       <c r="H11" t="n">
-        <v>1924.95</v>
+        <v>1464.7</v>
       </c>
       <c r="I11" t="n">
-        <v>19352.98</v>
+        <v>14866.68</v>
       </c>
       <c r="J11" t="n">
-        <v>99.59999999999999</v>
+        <v>75.81</v>
       </c>
       <c r="K11" t="n">
-        <v>1001.49</v>
+        <v>769.73</v>
       </c>
       <c r="L11" t="n">
-        <v>9.82</v>
+        <v>7.89</v>
       </c>
       <c r="M11" t="n">
-        <v>100.78</v>
+        <v>84.22</v>
       </c>
       <c r="N11" t="n">
         <v>0.77</v>
       </c>
       <c r="O11" t="n">
-        <v>12.8</v>
+        <v>9.6</v>
       </c>
       <c r="P11" t="n">
-        <v>44.32</v>
+        <v>30.8</v>
       </c>
       <c r="Q11" t="n">
-        <v>22.41</v>
+        <v>11.77</v>
       </c>
       <c r="R11" t="n">
-        <v>44.32</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="S11" t="n">
         <v>1</v>
       </c>
       <c r="T11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U11" t="n">
         <v>1</v>
@@ -1316,58 +1316,58 @@
         <v>60.27</v>
       </c>
       <c r="C12" t="n">
-        <v>11.72</v>
+        <v>13.06</v>
       </c>
       <c r="D12" t="n">
-        <v>11.72</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>11.72</v>
+        <v>13.06</v>
       </c>
       <c r="F12" t="n">
-        <v>11.72</v>
+        <v>13.06</v>
       </c>
       <c r="G12" t="n">
-        <v>13.39</v>
+        <v>21.1</v>
       </c>
       <c r="H12" t="n">
-        <v>1935.3</v>
+        <v>1486.67</v>
       </c>
       <c r="I12" t="n">
-        <v>19352.98</v>
+        <v>14866.68</v>
       </c>
       <c r="J12" t="n">
-        <v>100.15</v>
+        <v>76.97</v>
       </c>
       <c r="K12" t="n">
-        <v>1001.49</v>
+        <v>769.73</v>
       </c>
       <c r="L12" t="n">
-        <v>10.08</v>
+        <v>8.42</v>
       </c>
       <c r="M12" t="n">
-        <v>100.78</v>
+        <v>84.22</v>
       </c>
       <c r="N12" t="n">
-        <v>0.74</v>
+        <v>0.64</v>
       </c>
       <c r="O12" t="n">
-        <v>12.8</v>
+        <v>9.6</v>
       </c>
       <c r="P12" t="n">
-        <v>43.12</v>
+        <v>28.33</v>
       </c>
       <c r="Q12" t="n">
-        <v>21.89</v>
+        <v>11.05</v>
       </c>
       <c r="R12" t="n">
-        <v>43.12</v>
+        <v>5.83</v>
       </c>
       <c r="S12" t="n">
         <v>1</v>
       </c>
       <c r="T12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U12" t="n">
         <v>1</v>
@@ -1446,13 +1446,13 @@
         <v>65.5</v>
       </c>
       <c r="C2" t="n">
-        <v>51.36</v>
+        <v>41.7</v>
       </c>
       <c r="D2" t="n">
-        <v>13.27</v>
+        <v>22.92</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>30.15</v>
       </c>
       <c r="F2" t="n">
         <v>0.87</v>
@@ -1469,13 +1469,13 @@
         <v>64.52</v>
       </c>
       <c r="C3" t="n">
-        <v>50.04</v>
+        <v>41.94</v>
       </c>
       <c r="D3" t="n">
-        <v>14.48</v>
+        <v>22.58</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>35.32</v>
       </c>
       <c r="F3" t="n">
         <v>-0</v>
@@ -1492,13 +1492,13 @@
         <v>63.02</v>
       </c>
       <c r="C4" t="n">
-        <v>48.55</v>
+        <v>40.96</v>
       </c>
       <c r="D4" t="n">
-        <v>14.48</v>
+        <v>22.06</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>35.84</v>
       </c>
       <c r="F4" t="n">
         <v>-0</v>
@@ -1515,13 +1515,13 @@
         <v>61.66</v>
       </c>
       <c r="C5" t="n">
-        <v>47.19</v>
+        <v>40.08</v>
       </c>
       <c r="D5" t="n">
-        <v>14.48</v>
+        <v>21.58</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>36.32</v>
       </c>
       <c r="F5" t="n">
         <v>-0</v>
@@ -1538,13 +1538,13 @@
         <v>60.66</v>
       </c>
       <c r="C6" t="n">
-        <v>46.18</v>
+        <v>39.43</v>
       </c>
       <c r="D6" t="n">
-        <v>14.48</v>
+        <v>21.23</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>36.67</v>
       </c>
       <c r="F6" t="n">
         <v>-0</v>
@@ -1561,13 +1561,13 @@
         <v>59.61</v>
       </c>
       <c r="C7" t="n">
-        <v>45.13</v>
+        <v>38.75</v>
       </c>
       <c r="D7" t="n">
-        <v>14.48</v>
+        <v>20.86</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>37.04</v>
       </c>
       <c r="F7" t="n">
         <v>-0</v>
@@ -1584,19 +1584,19 @@
         <v>58.56</v>
       </c>
       <c r="C8" t="n">
-        <v>44.84</v>
+        <v>38.06</v>
       </c>
       <c r="D8" t="n">
-        <v>14.48</v>
+        <v>20.5</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>37.4</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.75</v>
+        <v>-0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.95</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="9">
@@ -1607,19 +1607,19 @@
         <v>57.51</v>
       </c>
       <c r="C9" t="n">
-        <v>44.94</v>
+        <v>37.38</v>
       </c>
       <c r="D9" t="n">
-        <v>12.57</v>
+        <v>20.13</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>30.13</v>
       </c>
       <c r="F9" t="n">
         <v>-0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.95</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="10">
@@ -1630,19 +1630,19 @@
         <v>56.46</v>
       </c>
       <c r="C10" t="n">
-        <v>44.84</v>
+        <v>36.7</v>
       </c>
       <c r="D10" t="n">
-        <v>11.66</v>
+        <v>19.76</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>26.88</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.05</v>
+        <v>-0</v>
       </c>
       <c r="G10" t="n">
-        <v>1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="11">
@@ -1653,16 +1653,16 @@
         <v>55.23</v>
       </c>
       <c r="C11" t="n">
-        <v>45.68</v>
+        <v>36.7</v>
       </c>
       <c r="D11" t="n">
-        <v>9.550000000000001</v>
+        <v>19.33</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>18.87</v>
       </c>
       <c r="F11" t="n">
-        <v>-0</v>
+        <v>-0.8</v>
       </c>
       <c r="G11" t="n">
         <v>1</v>
@@ -1678,19 +1678,19 @@
         <v>60.27</v>
       </c>
       <c r="C12" t="n">
-        <v>46.88</v>
+        <v>39.17</v>
       </c>
       <c r="D12" t="n">
-        <v>13.39</v>
+        <v>21.1</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>32.46</v>
       </c>
       <c r="F12" t="n">
         <v>0.01</v>
       </c>
       <c r="G12" t="n">
-        <v>0.51</v>
+        <v>0.28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>